<commit_message>
fix: replaced the updated excel
</commit_message>
<xml_diff>
--- a/Create-InstallLocation/LocInst.xlsx
+++ b/Create-InstallLocation/LocInst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mao8ct\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEF7A0D-7784-4265-B92C-5B8742E26EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE67B6C-9FCF-4280-BFE4-46D1D8351109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{841C4129-0CB3-4066-B34E-E8845E3509BE}"/>
   </bookViews>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D997F1F-30FE-4A2A-B694-A9178A4FC344}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,23 +451,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>4718301303</v>
+        <v>4718301787</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4718301617</v>
+        <v>4718301772</v>
       </c>
       <c r="B3" s="1">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4718301818</v>
+        <v>4728701146</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -475,31 +475,31 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4718301756</v>
+        <v>4718301609</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4718301787</v>
+        <v>4718301697</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4718301772</v>
+        <v>4718301461</v>
       </c>
       <c r="B7" s="1">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>4728701146</v>
+        <v>4718301814</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -507,23 +507,23 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4718301609</v>
+        <v>4718301815</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>4718301697</v>
+        <v>4718301805</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>4718301461</v>
+        <v>4718301819</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -531,49 +531,17 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>4718301814</v>
+        <v>4718301758</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>4718301815</v>
+        <v>4718301759</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>4718301805</v>
-      </c>
-      <c r="B14" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>4718301819</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>4718301758</v>
-      </c>
-      <c r="B16" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>4718301759</v>
-      </c>
-      <c r="B17" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>